<commit_message>
added all the parts required to recreate the device excluding the case
</commit_message>
<xml_diff>
--- a/Parts-required/bioGen-EMS-Parts-List.xlsx
+++ b/Parts-required/bioGen-EMS-Parts-List.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rakesh/Documents/Personal-and-Research/Research_Projects/EMS/bioGen-EMS/Parts-required/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D64C2F8-3A68-A343-A5C8-48CD9D26AA31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD1ADCD-81D1-384C-A715-F7D0221BE72C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41640" yWindow="2400" windowWidth="28040" windowHeight="17440" xr2:uid="{807E92EE-F4D5-BE48-86EB-4C690FDF2270}"/>
+    <workbookView xWindow="35840" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{807E92EE-F4D5-BE48-86EB-4C690FDF2270}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Electrical Parts" sheetId="1" r:id="rId1"/>
+    <sheet name="Stationary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,9 +34,167 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+  <si>
+    <t>Part Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price (USD)</t>
+  </si>
+  <si>
+    <t>Price (AUD)</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>SparkFun Solder-able Breadboard</t>
+  </si>
+  <si>
+    <t>A bare PCB that is the exact size as our regular breadboard with the same connections to pins and power rails. This board is especially useful for easy prototyping and hence why we chose this.</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>This breadboard size only supports a four-channel EMS device.</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/12070</t>
+  </si>
+  <si>
+    <t>Female PCB Header Connector</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The parts listed below are all required to build one single unit of bioGen-EMS device.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Qunqi-2-54mm-Straight-Connector-Arduino/dp/B07CGGSDWF/</t>
+  </si>
+  <si>
+    <t>$10 for 40 pieces</t>
+  </si>
+  <si>
+    <t>This is soldered onto the breadboard to mount the Arduino device.</t>
+  </si>
+  <si>
+    <t>2 pieces (max and you'll still be left with a lot of leftover)</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3379</t>
+  </si>
+  <si>
+    <t>Adafruit Feather 32u4 Bluefruit LE</t>
+  </si>
+  <si>
+    <t>This is the smallest bluetooth microcontroller with support for connecting a 3.7 V lithium ion battery available (at the time of documentation) to make the EMS device portable and customisable to meet individual needs.</t>
+  </si>
+  <si>
+    <t>Adafruit STEMMA Non-Latching Mini Relay</t>
+  </si>
+  <si>
+    <t>This is a very small relay, gets the job done and produces very low noise (also, solder free. Love this!)</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/4409</t>
+  </si>
+  <si>
+    <t>1 (recommend buying 2 just in case)</t>
+  </si>
+  <si>
+    <t>4 (recommend buying 6)</t>
+  </si>
+  <si>
+    <t>Lithium Ion Polymer Battery - 3.7v 350mAh</t>
+  </si>
+  <si>
+    <t>You can buy the device with pre-soldered headers (in-case you do not like soldering). :-) Also, this microcontroller charges the lithium ion battery you connect to it through the micro USB cable!</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2750</t>
+  </si>
+  <si>
+    <t>You can buy a bettery with a higher mAh value. For example, you will see me use a 2000 mAh battery in my video instructions.</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3893</t>
+  </si>
+  <si>
+    <t>STEMMA JST PH 3-Pin to Male Header Cable - 200mm</t>
+  </si>
+  <si>
+    <t>This cable will let you turn a JST PH 3-pin cable port into 3 individual wires with high-quality 0.1" male header plugs on the end.</t>
+  </si>
+  <si>
+    <t>The header pins will not matter much later as we will snap them off to solder them onto the breadboard.</t>
+  </si>
+  <si>
+    <t>Paper Tape (White)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.au/Aexit-Electrical-equipment-Adhesive-38ry728qf64/dp/B078LGQHQZ/</t>
+  </si>
+  <si>
+    <t>Jumper Cables</t>
+  </si>
+  <si>
+    <t>For connecting the relays and soldering them to the Sparkfun breadboards</t>
+  </si>
+  <si>
+    <t>1 Pack (More than enough)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.au/120pcs-Multicoloured-Dupont-Breadboard-arduino/dp/B01EV70C78/</t>
+  </si>
+  <si>
+    <t>Slide switch</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com.au/Aexit-electrical-Positions-Latching-10ry653qf391/dp/B07LFK8CN7/</t>
+  </si>
+  <si>
+    <t>I used a different slide switch. You can choose your own based on your aesthetic preferences.</t>
+  </si>
+  <si>
+    <t>This switch is used to turn on and turn off the bioGen-EMS circuit (to allow users to safely and easily kill in case of an uncomforable situation). For example, if they increased the intensity of the EMS too much by mistake when they are calibrating the electrodes themselves.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -43,13 +202,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -61,13 +248,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -380,12 +588,254 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA33AF02-5031-FE44-8338-F69E1C2DF1D2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="171" zoomScaleNormal="171" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="29" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="25" style="2" customWidth="1"/>
+    <col min="7" max="7" width="35.1640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4.95</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="5">
+        <v>31.95</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6.95</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5">
+        <v>5.95</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="7">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:G2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{69D964B7-7529-604D-9904-6423A660700E}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{4C12EE4A-EF71-C64C-A520-D3F09B738522}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{41015BB4-76AB-B24D-80D0-879C62BBEC11}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{4FAFBD91-1CCE-FA41-B550-9FF876F3046A}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{7BA6F516-18A0-4942-9E2F-86E6A6E32A5D}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{90BEF8DF-CA8C-6D4D-B6FD-FB8CE3C97E62}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{AD893BE2-F7C9-8042-9AC0-2B6FBED059AE}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{B52E1303-EE7C-5841-A7D7-43EB60C93EE5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D164EFB-793C-5544-8946-351E6301C4F7}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{BABC64A0-7ED4-554C-9DDA-0B9AC18F9EED}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made changes to the stationary list tab in the parts list document
</commit_message>
<xml_diff>
--- a/Parts-required/bioGen-EMS-Parts-List.xlsx
+++ b/Parts-required/bioGen-EMS-Parts-List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rakesh/Documents/Personal-and-Research/Research_Projects/EMS/bioGen-EMS/Parts-required/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD1ADCD-81D1-384C-A715-F7D0221BE72C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B6F06A-B02C-BB46-B76A-879DD44DF666}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{807E92EE-F4D5-BE48-86EB-4C690FDF2270}"/>
+    <workbookView xWindow="35840" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{807E92EE-F4D5-BE48-86EB-4C690FDF2270}"/>
   </bookViews>
   <sheets>
     <sheet name="Electrical Parts" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Part Name</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>This switch is used to turn on and turn off the bioGen-EMS circuit (to allow users to safely and easily kill in case of an uncomforable situation). For example, if they increased the intensity of the EMS too much by mistake when they are calibrating the electrodes themselves.</t>
+  </si>
+  <si>
+    <t>This will be used to add a label and number the relays for debugging and troubleshooting purposes.</t>
   </si>
 </sst>
 </file>
@@ -590,9 +593,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA33AF02-5031-FE44-8338-F69E1C2DF1D2}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="171" zoomScaleNormal="171" workbookViewId="0">
+    <sheetView zoomScale="171" zoomScaleNormal="171" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -803,14 +806,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D164EFB-793C-5544-8946-351E6301C4F7}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="85" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -830,6 +834,9 @@
       </c>
       <c r="B2" s="6" t="s">
         <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>